<commit_message>
H2 Import: Use IMP instead of IRE in process definition (temp bug fix)
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SYS_TTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SYS_TTechs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD200990-3C26-49CB-BEE0-DB18A62E4BC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F17E0C-C181-4785-8CEA-0CC774EB552C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CO2_backstop" sheetId="4" r:id="rId1"/>
@@ -1670,7 +1670,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="96">
   <si>
     <t>~FI_T</t>
   </si>
@@ -1919,9 +1919,6 @@
   </si>
   <si>
     <t>TRACO2N</t>
-  </si>
-  <si>
-    <t>IRE</t>
   </si>
   <si>
     <t>SUPH2GC</t>
@@ -2622,7 +2619,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B3:X40"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -3192,8 +3189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5009F66-579B-4F74-B783-938791DD3FCC}">
   <dimension ref="B1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3238,13 +3235,13 @@
         <v>5</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G2" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>93</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>94</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>17</v>
@@ -3253,7 +3250,7 @@
         <v>19</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L2" s="14" t="s">
         <v>6</v>
@@ -3295,7 +3292,7 @@
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I3" s="12" t="s">
         <v>58</v>
@@ -3304,7 +3301,7 @@
         <v>52</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L3" s="12" t="s">
         <v>56</v>
@@ -3342,16 +3339,16 @@
         <v/>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G4">
         <v>2030</v>
       </c>
       <c r="H4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I4">
         <v>2030</v>
@@ -3366,16 +3363,16 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5">
         <v>2050</v>
       </c>
       <c r="H5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K5">
         <f>6*1.2</f>
@@ -3516,19 +3513,19 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C18" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>87</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>

</xml_diff>

<commit_message>
Increased cost of H2, reduce ILED of BECCS to 0
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SYS_TTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SYS_TTechs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HannahD\Documents\GitHub\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F17E0C-C181-4785-8CEA-0CC774EB552C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAEC449-3030-4D2C-82C7-64D8702ABD5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4575" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CO2_backstop" sheetId="4" r:id="rId1"/>
@@ -2619,8 +2619,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B3:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3189,8 +3189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5009F66-579B-4F74-B783-938791DD3FCC}">
   <dimension ref="B1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3351,11 +3351,11 @@
         <v>94</v>
       </c>
       <c r="I4">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="K4">
-        <f>11*1.2</f>
-        <v>13.2</v>
+        <f>11*2</f>
+        <v>22</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -3375,8 +3375,8 @@
         <v>94</v>
       </c>
       <c r="K5">
-        <f>6*1.2</f>
-        <v>7.1999999999999993</v>
+        <f>6*2</f>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Rename DACS to be consistent with processes in SUP
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SYS_TTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SYS_TTechs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HannahD\Documents\GitHub\Irish-TIMES-model\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAEC449-3030-4D2C-82C7-64D8702ABD5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F35EFDE-0BAA-4978-93B1-682B3EEE7CD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CO2_backstop" sheetId="4" r:id="rId1"/>
@@ -1670,7 +1670,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="97">
   <si>
     <t>~FI_T</t>
   </si>
@@ -1876,9 +1876,6 @@
     <t>New Processes</t>
   </si>
   <si>
-    <t>DACS</t>
-  </si>
-  <si>
     <t>kt</t>
   </si>
   <si>
@@ -1958,6 +1955,12 @@
   </si>
   <si>
     <t>Import green H2 gaseous</t>
+  </si>
+  <si>
+    <t>SCO2DACS</t>
+  </si>
+  <si>
+    <t>CO2 Backstop process</t>
   </si>
 </sst>
 </file>
@@ -2619,8 +2622,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B3:X40"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2628,7 +2631,7 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
@@ -2679,7 +2682,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>4</v>
@@ -2794,11 +2797,11 @@
     <row r="9" spans="2:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" t="str">
         <f>C23</f>
-        <v>DACS</v>
+        <v>SCO2DACS</v>
       </c>
       <c r="C9" t="str">
         <f>D23</f>
-        <v>DACS</v>
+        <v>CO2 Backstop process</v>
       </c>
       <c r="E9" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,I31:I40)</f>
@@ -2945,19 +2948,19 @@
     </row>
     <row r="23" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B23" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="10" t="s">
+      <c r="F23" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>70</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
@@ -3018,7 +3021,7 @@
     </row>
     <row r="31" spans="2:24" x14ac:dyDescent="0.2">
       <c r="I31" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
@@ -3034,7 +3037,7 @@
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.2">
       <c r="I32" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
@@ -3050,7 +3053,7 @@
     </row>
     <row r="33" spans="9:24" x14ac:dyDescent="0.2">
       <c r="I33" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
@@ -3066,7 +3069,7 @@
     </row>
     <row r="34" spans="9:24" x14ac:dyDescent="0.2">
       <c r="I34" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M34" s="16"/>
       <c r="N34" s="16"/>
@@ -3082,7 +3085,7 @@
     </row>
     <row r="35" spans="9:24" x14ac:dyDescent="0.2">
       <c r="I35" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
@@ -3098,7 +3101,7 @@
     </row>
     <row r="36" spans="9:24" x14ac:dyDescent="0.2">
       <c r="I36" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M36" s="16"/>
       <c r="N36" s="16"/>
@@ -3114,7 +3117,7 @@
     </row>
     <row r="37" spans="9:24" x14ac:dyDescent="0.2">
       <c r="I37" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
@@ -3130,7 +3133,7 @@
     </row>
     <row r="38" spans="9:24" x14ac:dyDescent="0.2">
       <c r="I38" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
@@ -3146,7 +3149,7 @@
     </row>
     <row r="39" spans="9:24" x14ac:dyDescent="0.2">
       <c r="I39" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
@@ -3162,7 +3165,7 @@
     </row>
     <row r="40" spans="9:24" x14ac:dyDescent="0.2">
       <c r="I40" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M40" s="16"/>
       <c r="N40" s="16"/>
@@ -3189,8 +3192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5009F66-579B-4F74-B783-938791DD3FCC}">
   <dimension ref="B1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3226,7 +3229,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>3</v>
@@ -3235,13 +3238,13 @@
         <v>5</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>17</v>
@@ -3250,7 +3253,7 @@
         <v>19</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L2" s="14" t="s">
         <v>6</v>
@@ -3292,7 +3295,7 @@
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I3" s="12" t="s">
         <v>58</v>
@@ -3301,7 +3304,7 @@
         <v>52</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L3" s="12" t="s">
         <v>56</v>
@@ -3339,16 +3342,16 @@
         <v/>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G4">
         <v>2030</v>
       </c>
       <c r="H4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I4">
         <v>2025</v>
@@ -3363,16 +3366,16 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G5">
         <v>2050</v>
       </c>
       <c r="H5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K5">
         <f>6*2</f>
@@ -3513,19 +3516,19 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>

</xml_diff>